<commit_message>
All user stories - 2
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelResults/ScenarioStatus.xlsx
+++ b/src/test/java/ExcelResults/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
   <si>
     <t>Create Grade Level</t>
   </si>
@@ -83,6 +83,36 @@
   </si>
   <si>
     <t>07.09.22 16:07</t>
+  </si>
+  <si>
+    <t>07.09.22 18:02</t>
+  </si>
+  <si>
+    <t>07.09.22 18:29</t>
+  </si>
+  <si>
+    <t>07.09.22 18:50</t>
+  </si>
+  <si>
+    <t>07.09.22 18:39</t>
+  </si>
+  <si>
+    <t>07.09.22 18:59</t>
+  </si>
+  <si>
+    <t>07.09.22 18:52</t>
+  </si>
+  <si>
+    <t>07.09.22 18:16</t>
+  </si>
+  <si>
+    <t>07.09.22 18:55</t>
+  </si>
+  <si>
+    <t>07.09.22 18:20</t>
+  </si>
+  <si>
+    <t>07.09.22 18:43</t>
   </si>
 </sst>
 </file>
@@ -435,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="B4:E4"/>
@@ -572,6 +602,174 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tarafıma assigne edilmiş 3 senaryoyu da tamamladım, kontroller sonrası onaylanmasını talep ederim sayın leadim :)
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelResults/ScenarioStatus.xlsx
+++ b/src/test/java/ExcelResults/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="92">
   <si>
     <t>Create Grade Level</t>
   </si>
@@ -115,25 +115,187 @@
     <t>07.09.22 18:43</t>
   </si>
   <si>
-    <t>Create Fields</t>
-  </si>
-  <si>
-    <t>09.09.22 17:09</t>
-  </si>
-  <si>
-    <t>Edit Fields</t>
-  </si>
-  <si>
-    <t>09.09.22 17:30</t>
-  </si>
-  <si>
-    <t>09.09.22 22:33</t>
-  </si>
-  <si>
-    <t>09.09.22 22:01</t>
-  </si>
-  <si>
-    <t>09.09.22 22:23</t>
+    <t/>
+  </si>
+  <si>
+    <t>09.09.22 19:10</t>
+  </si>
+  <si>
+    <t>09.09.22 19:36</t>
+  </si>
+  <si>
+    <t>09.09.22 19:03</t>
+  </si>
+  <si>
+    <t>11.09.22 17:01</t>
+  </si>
+  <si>
+    <t>11.09.22 17:22</t>
+  </si>
+  <si>
+    <t>11.09.22 17:58</t>
+  </si>
+  <si>
+    <t>Add new Location</t>
+  </si>
+  <si>
+    <t>11.09.22 17:27</t>
+  </si>
+  <si>
+    <t>Edit new Location</t>
+  </si>
+  <si>
+    <t>11.09.22 17:44</t>
+  </si>
+  <si>
+    <t>11.09.22 17:43</t>
+  </si>
+  <si>
+    <t>11.09.22 17:15</t>
+  </si>
+  <si>
+    <t>11.09.22 17:47</t>
+  </si>
+  <si>
+    <t>11.09.22 17:02</t>
+  </si>
+  <si>
+    <t>11.09.22 17:59</t>
+  </si>
+  <si>
+    <t>11.09.22 17:23</t>
+  </si>
+  <si>
+    <t>11.09.22 17:34</t>
+  </si>
+  <si>
+    <t>11.09.22 17:55</t>
+  </si>
+  <si>
+    <t>11.09.22 17:03</t>
+  </si>
+  <si>
+    <t>11.09.22 17:19</t>
+  </si>
+  <si>
+    <t>11.09.22 17:49</t>
+  </si>
+  <si>
+    <t>11.09.22 17:39</t>
+  </si>
+  <si>
+    <t>11.09.22 18:02</t>
+  </si>
+  <si>
+    <t>Delete location</t>
+  </si>
+  <si>
+    <t>11.09.22 18:17</t>
+  </si>
+  <si>
+    <t>11.09.22 18:04</t>
+  </si>
+  <si>
+    <t>11.09.22 18:19</t>
+  </si>
+  <si>
+    <t>11.09.22 18:35</t>
+  </si>
+  <si>
+    <t>11.09.22 18:24</t>
+  </si>
+  <si>
+    <t>11.09.22 18:39</t>
+  </si>
+  <si>
+    <t>11.09.22 18:54</t>
+  </si>
+  <si>
+    <t>Add bankAccount</t>
+  </si>
+  <si>
+    <t>11.09.22 18:55</t>
+  </si>
+  <si>
+    <t>11.09.22 18:21</t>
+  </si>
+  <si>
+    <t>11.09.22 18:23</t>
+  </si>
+  <si>
+    <t>11.09.22 18:58</t>
+  </si>
+  <si>
+    <t>11.09.22 18:29</t>
+  </si>
+  <si>
+    <t>Edit bankAccount</t>
+  </si>
+  <si>
+    <t>11.09.22 18:53</t>
+  </si>
+  <si>
+    <t>11.09.22 19:24</t>
+  </si>
+  <si>
+    <t>11.09.22 19:43</t>
+  </si>
+  <si>
+    <t>11.09.22 19:40</t>
+  </si>
+  <si>
+    <t>11.09.22 19:20</t>
+  </si>
+  <si>
+    <t>11.09.22 20:29</t>
+  </si>
+  <si>
+    <t>11.09.22 20:44</t>
+  </si>
+  <si>
+    <t>11.09.22 20:37</t>
+  </si>
+  <si>
+    <t>11.09.22 20:55</t>
+  </si>
+  <si>
+    <t>11.09.22 20:53</t>
+  </si>
+  <si>
+    <t>11.09.22 20:51</t>
+  </si>
+  <si>
+    <t>11.09.22 21:04</t>
+  </si>
+  <si>
+    <t>11.09.22 21:21</t>
+  </si>
+  <si>
+    <t>11.09.22 21:37</t>
+  </si>
+  <si>
+    <t>11.09.22 21:55</t>
+  </si>
+  <si>
+    <t>11.09.22 21:52</t>
+  </si>
+  <si>
+    <t>11.09.22 21:20</t>
+  </si>
+  <si>
+    <t>Delete bankAccount</t>
+  </si>
+  <si>
+    <t>11.09.22 21:50</t>
+  </si>
+  <si>
+    <t>11.09.22 21:13</t>
+  </si>
+  <si>
+    <t>11.09.22 21:31</t>
+  </si>
+  <si>
+    <t>11.09.22 21:47</t>
   </si>
 </sst>
 </file>
@@ -486,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="B4:E4"/>
@@ -807,21 +969,21 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -830,35 +992,1001 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
       <c r="D26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>63</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>63</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>63</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>63</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>69</v>
+      </c>
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>87</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>63</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>69</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extent Report & Master Report
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelResults/ScenarioStatus.xlsx
+++ b/src/test/java/ExcelResults/ScenarioStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="219">
   <si>
     <t>Create Subject Categories</t>
   </si>
@@ -206,6 +206,477 @@
   </si>
   <si>
     <t>14.09.22 18:26</t>
+  </si>
+  <si>
+    <t>Add new Position</t>
+  </si>
+  <si>
+    <t>15.09.22 12:24</t>
+  </si>
+  <si>
+    <t>Edit Exist Position</t>
+  </si>
+  <si>
+    <t>15.09.22 12:00</t>
+  </si>
+  <si>
+    <t>Delete Exist Position</t>
+  </si>
+  <si>
+    <t>15.09.22 12:37</t>
+  </si>
+  <si>
+    <t>15.09.22 13:49</t>
+  </si>
+  <si>
+    <t>15.09.22 13:28</t>
+  </si>
+  <si>
+    <t>15.09.22 13:01</t>
+  </si>
+  <si>
+    <t>15.09.22 13:05</t>
+  </si>
+  <si>
+    <t>15.09.22 13:02</t>
+  </si>
+  <si>
+    <t>15.09.22 13:04</t>
+  </si>
+  <si>
+    <t>15.09.22 13:30</t>
+  </si>
+  <si>
+    <t>15.09.22 13:56</t>
+  </si>
+  <si>
+    <t>15.09.22 14:41</t>
+  </si>
+  <si>
+    <t>15.09.22 14:47</t>
+  </si>
+  <si>
+    <t>15.09.22 14:13</t>
+  </si>
+  <si>
+    <t>15.09.22 14:33</t>
+  </si>
+  <si>
+    <t>15.09.22 14:25</t>
+  </si>
+  <si>
+    <t>15.09.22 14:51</t>
+  </si>
+  <si>
+    <t>15.09.22 14:53</t>
+  </si>
+  <si>
+    <t>15.09.22 14:45</t>
+  </si>
+  <si>
+    <t>15.09.22 14:05</t>
+  </si>
+  <si>
+    <t>15.09.22 14:50</t>
+  </si>
+  <si>
+    <t>15.09.22 14:12</t>
+  </si>
+  <si>
+    <t>15.09.22 14:36</t>
+  </si>
+  <si>
+    <t>15.09.22 15:10</t>
+  </si>
+  <si>
+    <t>15.09.22 15:31</t>
+  </si>
+  <si>
+    <t>15.09.22 15:03</t>
+  </si>
+  <si>
+    <t>15.09.22 15:22</t>
+  </si>
+  <si>
+    <t>15.09.22 15:17</t>
+  </si>
+  <si>
+    <t>15.09.22 15:40</t>
+  </si>
+  <si>
+    <t>15.09.22 15:04</t>
+  </si>
+  <si>
+    <t>15.09.22 15:58</t>
+  </si>
+  <si>
+    <t>15.09.22 15:19</t>
+  </si>
+  <si>
+    <t>15.09.22 15:07</t>
+  </si>
+  <si>
+    <t>15.09.22 15:34</t>
+  </si>
+  <si>
+    <t>15.09.22 15:54</t>
+  </si>
+  <si>
+    <t>15.09.22 15:21</t>
+  </si>
+  <si>
+    <t>15.09.22 15:45</t>
+  </si>
+  <si>
+    <t>15.09.22 17:32</t>
+  </si>
+  <si>
+    <t>15.09.22 17:56</t>
+  </si>
+  <si>
+    <t>15.09.22 17:48</t>
+  </si>
+  <si>
+    <t>15.09.22 17:50</t>
+  </si>
+  <si>
+    <t>15.09.22 17:15</t>
+  </si>
+  <si>
+    <t>15.09.22 17:05</t>
+  </si>
+  <si>
+    <t>15.09.22 17:21</t>
+  </si>
+  <si>
+    <t>15.09.22 17:42</t>
+  </si>
+  <si>
+    <t>15.09.22 17:03</t>
+  </si>
+  <si>
+    <t>15.09.22 17:59</t>
+  </si>
+  <si>
+    <t>15.09.22 17:46</t>
+  </si>
+  <si>
+    <t>15.09.22 17:12</t>
+  </si>
+  <si>
+    <t>15.09.22 17:33</t>
+  </si>
+  <si>
+    <t>15.09.22 18:01</t>
+  </si>
+  <si>
+    <t>15.09.22 18:39</t>
+  </si>
+  <si>
+    <t>15.09.22 18:23</t>
+  </si>
+  <si>
+    <t>15.09.22 18:32</t>
+  </si>
+  <si>
+    <t>15.09.22 18:29</t>
+  </si>
+  <si>
+    <t>15.09.22 18:04</t>
+  </si>
+  <si>
+    <t>15.09.22 18:14</t>
+  </si>
+  <si>
+    <t>15.09.22 18:44</t>
+  </si>
+  <si>
+    <t>15.09.22 18:06</t>
+  </si>
+  <si>
+    <t>16.09.22 14:07</t>
+  </si>
+  <si>
+    <t>16.09.22 14:45</t>
+  </si>
+  <si>
+    <t>16.09.22 14:23</t>
+  </si>
+  <si>
+    <t>16.09.22 14:59</t>
+  </si>
+  <si>
+    <t>16.09.22 14:51</t>
+  </si>
+  <si>
+    <t>16.09.22 14:29</t>
+  </si>
+  <si>
+    <t>16.09.22 14:58</t>
+  </si>
+  <si>
+    <t>16.09.22 14:36</t>
+  </si>
+  <si>
+    <t>16.09.22 14:19</t>
+  </si>
+  <si>
+    <t>16.09.22 14:54</t>
+  </si>
+  <si>
+    <t>16.09.22 14:12</t>
+  </si>
+  <si>
+    <t>16.09.22 14:57</t>
+  </si>
+  <si>
+    <t>16.09.22 14:56</t>
+  </si>
+  <si>
+    <t>16.09.22 14:24</t>
+  </si>
+  <si>
+    <t>16.09.22 14:52</t>
+  </si>
+  <si>
+    <t>16.09.22 14:30</t>
+  </si>
+  <si>
+    <t>16.09.22 15:50</t>
+  </si>
+  <si>
+    <t>16.09.22 15:53</t>
+  </si>
+  <si>
+    <t>16.09.22 15:37</t>
+  </si>
+  <si>
+    <t>16.09.22 15:32</t>
+  </si>
+  <si>
+    <t>16.09.22 15:18</t>
+  </si>
+  <si>
+    <t>16.09.22 15:44</t>
+  </si>
+  <si>
+    <t>16.09.22 15:19</t>
+  </si>
+  <si>
+    <t>16.09.22 15:17</t>
+  </si>
+  <si>
+    <t>16.09.22 15:39</t>
+  </si>
+  <si>
+    <t>16.09.22 15:59</t>
+  </si>
+  <si>
+    <t>16.09.22 15:34</t>
+  </si>
+  <si>
+    <t>16.09.22 15:57</t>
+  </si>
+  <si>
+    <t>16.09.22 15:20</t>
+  </si>
+  <si>
+    <t>16.09.22 15:05</t>
+  </si>
+  <si>
+    <t>16.09.22 15:28</t>
+  </si>
+  <si>
+    <t>16.09.22 15:48</t>
+  </si>
+  <si>
+    <t>16.09.22 17:11</t>
+  </si>
+  <si>
+    <t>16.09.22 17:35</t>
+  </si>
+  <si>
+    <t>16.09.22 17:56</t>
+  </si>
+  <si>
+    <t>16.09.22 17:21</t>
+  </si>
+  <si>
+    <t>16.09.22 17:17</t>
+  </si>
+  <si>
+    <t>16.09.22 17:54</t>
+  </si>
+  <si>
+    <t>16.09.22 17:42</t>
+  </si>
+  <si>
+    <t>16.09.22 17:08</t>
+  </si>
+  <si>
+    <t>16.09.22 17:27</t>
+  </si>
+  <si>
+    <t>16.09.22 17:50</t>
+  </si>
+  <si>
+    <t>16.09.22 17:09</t>
+  </si>
+  <si>
+    <t>16.09.22 17:49</t>
+  </si>
+  <si>
+    <t>16.09.22 17:12</t>
+  </si>
+  <si>
+    <t>16.09.22 17:20</t>
+  </si>
+  <si>
+    <t>16.09.22 17:45</t>
+  </si>
+  <si>
+    <t>16.09.22 17:07</t>
+  </si>
+  <si>
+    <t>16.09.22 17:47</t>
+  </si>
+  <si>
+    <t>16.09.22 17:13</t>
+  </si>
+  <si>
+    <t>16.09.22 17:37</t>
+  </si>
+  <si>
+    <t>16.09.22 17:41</t>
+  </si>
+  <si>
+    <t>16.09.22 17:33</t>
+  </si>
+  <si>
+    <t>16.09.22 17:15</t>
+  </si>
+  <si>
+    <t>16.09.22 17:16</t>
+  </si>
+  <si>
+    <t>16.09.22 17:59</t>
+  </si>
+  <si>
+    <t>16.09.22 17:00</t>
+  </si>
+  <si>
+    <t>16.09.22 17:52</t>
+  </si>
+  <si>
+    <t>16.09.22 17:18</t>
+  </si>
+  <si>
+    <t>16.09.22 17:48</t>
+  </si>
+  <si>
+    <t>16.09.22 17:14</t>
+  </si>
+  <si>
+    <t>16.09.22 17:05</t>
+  </si>
+  <si>
+    <t>16.09.22 17:06</t>
+  </si>
+  <si>
+    <t>16.09.22 17:34</t>
+  </si>
+  <si>
+    <t>16.09.22 17:29</t>
+  </si>
+  <si>
+    <t>16.09.22 17:36</t>
+  </si>
+  <si>
+    <t>16.09.22 17:38</t>
+  </si>
+  <si>
+    <t>16.09.22 17:58</t>
+  </si>
+  <si>
+    <t>16.09.22 18:15</t>
+  </si>
+  <si>
+    <t>16.09.22 18:51</t>
+  </si>
+  <si>
+    <t>16.09.22 18:02</t>
+  </si>
+  <si>
+    <t>16.09.22 18:12</t>
+  </si>
+  <si>
+    <t>16.09.22 18:29</t>
+  </si>
+  <si>
+    <t>16.09.22 18:49</t>
+  </si>
+  <si>
+    <t>16.09.22 18:23</t>
+  </si>
+  <si>
+    <t>16.09.22 18:17</t>
+  </si>
+  <si>
+    <t>16.09.22 18:41</t>
+  </si>
+  <si>
+    <t>16.09.22 18:11</t>
+  </si>
+  <si>
+    <t>16.09.22 18:37</t>
+  </si>
+  <si>
+    <t>16.09.22 18:59</t>
+  </si>
+  <si>
+    <t>16.09.22 18:32</t>
+  </si>
+  <si>
+    <t>16.09.22 18:31</t>
+  </si>
+  <si>
+    <t>16.09.22 18:52</t>
+  </si>
+  <si>
+    <t>16.09.22 18:14</t>
+  </si>
+  <si>
+    <t>16.09.22 18:50</t>
+  </si>
+  <si>
+    <t>16.09.22 18:58</t>
+  </si>
+  <si>
+    <t>16.09.22 18:20</t>
+  </si>
+  <si>
+    <t>16.09.22 18:46</t>
+  </si>
+  <si>
+    <t>16.09.22 18:18</t>
+  </si>
+  <si>
+    <t>16.09.22 18:43</t>
+  </si>
+  <si>
+    <t>16.09.22 18:03</t>
+  </si>
+  <si>
+    <t>16.09.22 18:34</t>
+  </si>
+  <si>
+    <t>16.09.22 18:56</t>
+  </si>
+  <si>
+    <t>16.09.22 18:16</t>
+  </si>
+  <si>
+    <t>16.09.22 18:38</t>
   </si>
 </sst>
 </file>
@@ -558,7 +1029,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
@@ -1423,6 +1894,2576 @@
         <v>61</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>62</v>
+      </c>
+      <c r="B77" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>64</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>64</v>
+      </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>62</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>64</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>62</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>64</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>66</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>62</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>66</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>62</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>64</v>
+      </c>
+      <c r="B93" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>62</v>
+      </c>
+      <c r="B95" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>64</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D96" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>62</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>66</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>62</v>
+      </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>64</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>66</v>
+      </c>
+      <c r="B103" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>62</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>64</v>
+      </c>
+      <c r="B105" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>66</v>
+      </c>
+      <c r="B106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>62</v>
+      </c>
+      <c r="B107" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>64</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>62</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>64</v>
+      </c>
+      <c r="B111" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>62</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>64</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>66</v>
+      </c>
+      <c r="B114" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>62</v>
+      </c>
+      <c r="B115" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>64</v>
+      </c>
+      <c r="B116" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>66</v>
+      </c>
+      <c r="B117" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>62</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>64</v>
+      </c>
+      <c r="B119" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>66</v>
+      </c>
+      <c r="B120" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>62</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>64</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>66</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>62</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>64</v>
+      </c>
+      <c r="B125" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+      <c r="D125" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>66</v>
+      </c>
+      <c r="B126" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+      <c r="D126" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>62</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+      <c r="D127" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>62</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>64</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>66</v>
+      </c>
+      <c r="B130" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" t="s">
+        <v>2</v>
+      </c>
+      <c r="D130" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>62</v>
+      </c>
+      <c r="B131" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+      <c r="D131" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>64</v>
+      </c>
+      <c r="B132" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>66</v>
+      </c>
+      <c r="B133" t="s">
+        <v>15</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>62</v>
+      </c>
+      <c r="B134" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>64</v>
+      </c>
+      <c r="B135" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>62</v>
+      </c>
+      <c r="B136" t="s">
+        <v>15</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>64</v>
+      </c>
+      <c r="B137" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>62</v>
+      </c>
+      <c r="B138" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" t="s">
+        <v>2</v>
+      </c>
+      <c r="D138" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>64</v>
+      </c>
+      <c r="B139" t="s">
+        <v>15</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>66</v>
+      </c>
+      <c r="B140" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>62</v>
+      </c>
+      <c r="B141" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>64</v>
+      </c>
+      <c r="B142" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+      <c r="D142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>66</v>
+      </c>
+      <c r="B143" t="s">
+        <v>15</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+      <c r="D143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>62</v>
+      </c>
+      <c r="B144" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" t="s">
+        <v>2</v>
+      </c>
+      <c r="D144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>62</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1</v>
+      </c>
+      <c r="C145" t="s">
+        <v>2</v>
+      </c>
+      <c r="D145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>64</v>
+      </c>
+      <c r="B146" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2</v>
+      </c>
+      <c r="D146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>66</v>
+      </c>
+      <c r="B147" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+      <c r="D147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>62</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s">
+        <v>2</v>
+      </c>
+      <c r="D148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>64</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>66</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>62</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>64</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>2</v>
+      </c>
+      <c r="D152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>66</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>62</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>64</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>66</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>62</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" t="s">
+        <v>2</v>
+      </c>
+      <c r="D157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>64</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>2</v>
+      </c>
+      <c r="D158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>66</v>
+      </c>
+      <c r="B159" t="s">
+        <v>15</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2</v>
+      </c>
+      <c r="D159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>62</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>64</v>
+      </c>
+      <c r="B161" t="s">
+        <v>15</v>
+      </c>
+      <c r="C161" t="s">
+        <v>2</v>
+      </c>
+      <c r="D161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>66</v>
+      </c>
+      <c r="B162" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" t="s">
+        <v>2</v>
+      </c>
+      <c r="D162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>62</v>
+      </c>
+      <c r="B163" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>64</v>
+      </c>
+      <c r="B164" t="s">
+        <v>15</v>
+      </c>
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>62</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>64</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+      <c r="D166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>66</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" t="s">
+        <v>2</v>
+      </c>
+      <c r="D167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>62</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>2</v>
+      </c>
+      <c r="D168" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>64</v>
+      </c>
+      <c r="B169" t="s">
+        <v>15</v>
+      </c>
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>62</v>
+      </c>
+      <c r="B170" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>64</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>66</v>
+      </c>
+      <c r="B172" t="s">
+        <v>15</v>
+      </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>66</v>
+      </c>
+      <c r="B173" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>62</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" t="s">
+        <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>64</v>
+      </c>
+      <c r="B175" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>62</v>
+      </c>
+      <c r="B176" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>66</v>
+      </c>
+      <c r="B177" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" t="s">
+        <v>2</v>
+      </c>
+      <c r="D177" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>64</v>
+      </c>
+      <c r="B178" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" t="s">
+        <v>2</v>
+      </c>
+      <c r="D178" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>62</v>
+      </c>
+      <c r="B179" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" t="s">
+        <v>2</v>
+      </c>
+      <c r="D179" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>62</v>
+      </c>
+      <c r="B180" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180"/>
+      <c r="D180" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>64</v>
+      </c>
+      <c r="B181" t="s">
+        <v>15</v>
+      </c>
+      <c r="C181"/>
+      <c r="D181" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>66</v>
+      </c>
+      <c r="B182" t="s">
+        <v>15</v>
+      </c>
+      <c r="C182"/>
+      <c r="D182" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>62</v>
+      </c>
+      <c r="B183" t="s">
+        <v>15</v>
+      </c>
+      <c r="C183" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>64</v>
+      </c>
+      <c r="B184" t="s">
+        <v>15</v>
+      </c>
+      <c r="C184" t="s">
+        <v>2</v>
+      </c>
+      <c r="D184" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>66</v>
+      </c>
+      <c r="B185" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" t="s">
+        <v>2</v>
+      </c>
+      <c r="D185" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>64</v>
+      </c>
+      <c r="B186" t="s">
+        <v>15</v>
+      </c>
+      <c r="C186" t="s">
+        <v>2</v>
+      </c>
+      <c r="D186" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>66</v>
+      </c>
+      <c r="B187" t="s">
+        <v>15</v>
+      </c>
+      <c r="C187" t="s">
+        <v>2</v>
+      </c>
+      <c r="D187" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>62</v>
+      </c>
+      <c r="B188" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188" t="s">
+        <v>2</v>
+      </c>
+      <c r="D188" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>64</v>
+      </c>
+      <c r="B189" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" t="s">
+        <v>2</v>
+      </c>
+      <c r="D189" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>66</v>
+      </c>
+      <c r="B190" t="s">
+        <v>15</v>
+      </c>
+      <c r="C190" t="s">
+        <v>2</v>
+      </c>
+      <c r="D190" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>62</v>
+      </c>
+      <c r="B191" t="s">
+        <v>15</v>
+      </c>
+      <c r="C191" t="s">
+        <v>2</v>
+      </c>
+      <c r="D191" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>64</v>
+      </c>
+      <c r="B192" t="s">
+        <v>15</v>
+      </c>
+      <c r="C192" t="s">
+        <v>2</v>
+      </c>
+      <c r="D192" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>66</v>
+      </c>
+      <c r="B193" t="s">
+        <v>15</v>
+      </c>
+      <c r="C193" t="s">
+        <v>2</v>
+      </c>
+      <c r="D193" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>62</v>
+      </c>
+      <c r="B194" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" t="s">
+        <v>2</v>
+      </c>
+      <c r="D194" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>62</v>
+      </c>
+      <c r="B195" t="s">
+        <v>15</v>
+      </c>
+      <c r="C195" t="s">
+        <v>2</v>
+      </c>
+      <c r="D195" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>64</v>
+      </c>
+      <c r="B196" t="s">
+        <v>15</v>
+      </c>
+      <c r="C196" t="s">
+        <v>2</v>
+      </c>
+      <c r="D196" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>64</v>
+      </c>
+      <c r="B197" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197" t="s">
+        <v>2</v>
+      </c>
+      <c r="D197" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>62</v>
+      </c>
+      <c r="B198" t="s">
+        <v>15</v>
+      </c>
+      <c r="C198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D198" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>64</v>
+      </c>
+      <c r="B199" t="s">
+        <v>15</v>
+      </c>
+      <c r="C199" t="s">
+        <v>2</v>
+      </c>
+      <c r="D199" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>64</v>
+      </c>
+      <c r="B200" t="s">
+        <v>15</v>
+      </c>
+      <c r="C200" t="s">
+        <v>2</v>
+      </c>
+      <c r="D200" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>62</v>
+      </c>
+      <c r="B201" t="s">
+        <v>1</v>
+      </c>
+      <c r="C201" t="s">
+        <v>2</v>
+      </c>
+      <c r="D201" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>62</v>
+      </c>
+      <c r="B202" t="s">
+        <v>15</v>
+      </c>
+      <c r="C202" t="s">
+        <v>2</v>
+      </c>
+      <c r="D202" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203" t="s">
+        <v>15</v>
+      </c>
+      <c r="C203" t="s">
+        <v>2</v>
+      </c>
+      <c r="D203" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>66</v>
+      </c>
+      <c r="B204" t="s">
+        <v>15</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2</v>
+      </c>
+      <c r="D204" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>62</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C205" t="s">
+        <v>2</v>
+      </c>
+      <c r="D205" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>64</v>
+      </c>
+      <c r="B206" t="s">
+        <v>15</v>
+      </c>
+      <c r="C206" t="s">
+        <v>2</v>
+      </c>
+      <c r="D206" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>62</v>
+      </c>
+      <c r="B207" t="s">
+        <v>15</v>
+      </c>
+      <c r="C207" t="s">
+        <v>2</v>
+      </c>
+      <c r="D207" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>66</v>
+      </c>
+      <c r="B208" t="s">
+        <v>15</v>
+      </c>
+      <c r="C208" t="s">
+        <v>2</v>
+      </c>
+      <c r="D208" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>64</v>
+      </c>
+      <c r="B209" t="s">
+        <v>15</v>
+      </c>
+      <c r="C209" t="s">
+        <v>2</v>
+      </c>
+      <c r="D209" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>66</v>
+      </c>
+      <c r="B210" t="s">
+        <v>15</v>
+      </c>
+      <c r="C210" t="s">
+        <v>2</v>
+      </c>
+      <c r="D210" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>62</v>
+      </c>
+      <c r="B211" t="s">
+        <v>15</v>
+      </c>
+      <c r="C211" t="s">
+        <v>2</v>
+      </c>
+      <c r="D211" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>62</v>
+      </c>
+      <c r="B212" t="s">
+        <v>15</v>
+      </c>
+      <c r="C212" t="s">
+        <v>2</v>
+      </c>
+      <c r="D212" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>64</v>
+      </c>
+      <c r="B213" t="s">
+        <v>15</v>
+      </c>
+      <c r="C213" t="s">
+        <v>2</v>
+      </c>
+      <c r="D213" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>64</v>
+      </c>
+      <c r="B214" t="s">
+        <v>15</v>
+      </c>
+      <c r="C214" t="s">
+        <v>2</v>
+      </c>
+      <c r="D214" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>62</v>
+      </c>
+      <c r="B215" t="s">
+        <v>15</v>
+      </c>
+      <c r="C215" t="s">
+        <v>2</v>
+      </c>
+      <c r="D215" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>64</v>
+      </c>
+      <c r="B216" t="s">
+        <v>15</v>
+      </c>
+      <c r="C216" t="s">
+        <v>2</v>
+      </c>
+      <c r="D216" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>66</v>
+      </c>
+      <c r="B217" t="s">
+        <v>15</v>
+      </c>
+      <c r="C217" t="s">
+        <v>2</v>
+      </c>
+      <c r="D217" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>66</v>
+      </c>
+      <c r="B218" t="s">
+        <v>15</v>
+      </c>
+      <c r="C218" t="s">
+        <v>2</v>
+      </c>
+      <c r="D218" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>62</v>
+      </c>
+      <c r="B219" t="s">
+        <v>1</v>
+      </c>
+      <c r="C219" t="s">
+        <v>2</v>
+      </c>
+      <c r="D219" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>64</v>
+      </c>
+      <c r="B220" t="s">
+        <v>15</v>
+      </c>
+      <c r="C220" t="s">
+        <v>2</v>
+      </c>
+      <c r="D220" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>66</v>
+      </c>
+      <c r="B221" t="s">
+        <v>15</v>
+      </c>
+      <c r="C221" t="s">
+        <v>2</v>
+      </c>
+      <c r="D221" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>62</v>
+      </c>
+      <c r="B222" t="s">
+        <v>1</v>
+      </c>
+      <c r="C222" t="s">
+        <v>2</v>
+      </c>
+      <c r="D222" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>64</v>
+      </c>
+      <c r="B223" t="s">
+        <v>15</v>
+      </c>
+      <c r="C223" t="s">
+        <v>2</v>
+      </c>
+      <c r="D223" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>66</v>
+      </c>
+      <c r="B224" t="s">
+        <v>15</v>
+      </c>
+      <c r="C224" t="s">
+        <v>2</v>
+      </c>
+      <c r="D224" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>62</v>
+      </c>
+      <c r="B225" t="s">
+        <v>1</v>
+      </c>
+      <c r="C225" t="s">
+        <v>2</v>
+      </c>
+      <c r="D225" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>64</v>
+      </c>
+      <c r="B226" t="s">
+        <v>15</v>
+      </c>
+      <c r="C226" t="s">
+        <v>2</v>
+      </c>
+      <c r="D226" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>66</v>
+      </c>
+      <c r="B227" t="s">
+        <v>15</v>
+      </c>
+      <c r="C227" t="s">
+        <v>2</v>
+      </c>
+      <c r="D227" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>62</v>
+      </c>
+      <c r="B228" t="s">
+        <v>1</v>
+      </c>
+      <c r="C228" t="s">
+        <v>2</v>
+      </c>
+      <c r="D228" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>64</v>
+      </c>
+      <c r="B229" t="s">
+        <v>15</v>
+      </c>
+      <c r="C229" t="s">
+        <v>2</v>
+      </c>
+      <c r="D229" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>66</v>
+      </c>
+      <c r="B230" t="s">
+        <v>15</v>
+      </c>
+      <c r="C230" t="s">
+        <v>2</v>
+      </c>
+      <c r="D230" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>62</v>
+      </c>
+      <c r="B231" t="s">
+        <v>1</v>
+      </c>
+      <c r="C231" t="s">
+        <v>2</v>
+      </c>
+      <c r="D231" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>64</v>
+      </c>
+      <c r="B232" t="s">
+        <v>15</v>
+      </c>
+      <c r="C232" t="s">
+        <v>2</v>
+      </c>
+      <c r="D232" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>66</v>
+      </c>
+      <c r="B233" t="s">
+        <v>15</v>
+      </c>
+      <c r="C233" t="s">
+        <v>2</v>
+      </c>
+      <c r="D233" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>62</v>
+      </c>
+      <c r="B234" t="s">
+        <v>1</v>
+      </c>
+      <c r="C234" t="s">
+        <v>2</v>
+      </c>
+      <c r="D234" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>64</v>
+      </c>
+      <c r="B235" t="s">
+        <v>15</v>
+      </c>
+      <c r="C235" t="s">
+        <v>2</v>
+      </c>
+      <c r="D235" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>66</v>
+      </c>
+      <c r="B236" t="s">
+        <v>15</v>
+      </c>
+      <c r="C236" t="s">
+        <v>2</v>
+      </c>
+      <c r="D236" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>62</v>
+      </c>
+      <c r="B237" t="s">
+        <v>1</v>
+      </c>
+      <c r="C237" t="s">
+        <v>2</v>
+      </c>
+      <c r="D237" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>64</v>
+      </c>
+      <c r="B238" t="s">
+        <v>1</v>
+      </c>
+      <c r="C238" t="s">
+        <v>2</v>
+      </c>
+      <c r="D238" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>66</v>
+      </c>
+      <c r="B239" t="s">
+        <v>1</v>
+      </c>
+      <c r="C239" t="s">
+        <v>2</v>
+      </c>
+      <c r="D239" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>62</v>
+      </c>
+      <c r="B240" t="s">
+        <v>1</v>
+      </c>
+      <c r="C240" t="s">
+        <v>2</v>
+      </c>
+      <c r="D240" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>64</v>
+      </c>
+      <c r="B241" t="s">
+        <v>1</v>
+      </c>
+      <c r="C241" t="s">
+        <v>2</v>
+      </c>
+      <c r="D241" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>66</v>
+      </c>
+      <c r="B242" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242" t="s">
+        <v>2</v>
+      </c>
+      <c r="D242" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>62</v>
+      </c>
+      <c r="B243" t="s">
+        <v>1</v>
+      </c>
+      <c r="C243" t="s">
+        <v>2</v>
+      </c>
+      <c r="D243" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>64</v>
+      </c>
+      <c r="B244" t="s">
+        <v>1</v>
+      </c>
+      <c r="C244" t="s">
+        <v>2</v>
+      </c>
+      <c r="D244" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>66</v>
+      </c>
+      <c r="B245" t="s">
+        <v>1</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2</v>
+      </c>
+      <c r="D245" t="s">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>